<commit_message>
Add 2021 data and 1-year race/age statewide trends to CCB
</commit_message>
<xml_diff>
--- a/myCCB/Standards/sdohLink.xlsx
+++ b/myCCB/Standards/sdohLink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624468F0-E687-45DB-9153-3290B403B351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C659D7-CBA4-4685-BC31-B14559F7E169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,6 +228,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -253,8 +260,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,7 +580,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +622,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -771,7 +779,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
@@ -791,7 +799,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">

</xml_diff>

<commit_message>
Clean upstream folder; Sept 2022 CCB update; Sonoma age-adjust examples
</commit_message>
<xml_diff>
--- a/myCCB/Standards/sdohLink.xlsx
+++ b/myCCB/Standards/sdohLink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C659D7-CBA4-4685-BC31-B14559F7E169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2FC1E1-80FA-40E3-9080-0A5F93451F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
+    <workbookView xWindow="255" yWindow="630" windowWidth="21600" windowHeight="11385" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
   <si>
     <t>hpi2score</t>
   </si>
@@ -151,9 +151,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>HPI Score</t>
-  </si>
-  <si>
     <t>Insured</t>
   </si>
   <si>
@@ -175,18 +172,9 @@
     <t>Plumbing</t>
   </si>
   <si>
-    <t>Park Access</t>
-  </si>
-  <si>
     <t>Internet</t>
   </si>
   <si>
-    <t>Crowded Household</t>
-  </si>
-  <si>
-    <t>Limited English</t>
-  </si>
-  <si>
     <t>hsGradAndBelow</t>
   </si>
   <si>
@@ -212,13 +200,118 @@
   </si>
   <si>
     <t>sdohName</t>
+  </si>
+  <si>
+    <t>inSCODA</t>
+  </si>
+  <si>
+    <t>redline</t>
+  </si>
+  <si>
+    <t>Historically Redlined</t>
+  </si>
+  <si>
+    <t>redlined</t>
+  </si>
+  <si>
+    <t>Percentage of households with interest, dividends, or net rental income in the past 12 months</t>
+  </si>
+  <si>
+    <t>extraincome</t>
+  </si>
+  <si>
+    <t>extraIncome</t>
+  </si>
+  <si>
+    <t>foodAffordability</t>
+  </si>
+  <si>
+    <t>affordfood</t>
+  </si>
+  <si>
+    <t>voting</t>
+  </si>
+  <si>
+    <t>Percentage of registered voters voting in the 2020 general election</t>
+  </si>
+  <si>
+    <t>Voted</t>
+  </si>
+  <si>
+    <t>voted</t>
+  </si>
+  <si>
+    <t>commute</t>
+  </si>
+  <si>
+    <t>Commute</t>
+  </si>
+  <si>
+    <t>Percentage of workers (16 years and older) who commute to work by transit, walking, or cycling</t>
+  </si>
+  <si>
+    <t>rentsevere</t>
+  </si>
+  <si>
+    <t>rent50severe</t>
+  </si>
+  <si>
+    <t>Percentage of low income renter households with housing costs exceeding 50% of income</t>
+  </si>
+  <si>
+    <t>pm25</t>
+  </si>
+  <si>
+    <t>PM25</t>
+  </si>
+  <si>
+    <t>Annual mean concentration of PM2.5 (μg/m3)</t>
+  </si>
+  <si>
+    <t>commute2</t>
+  </si>
+  <si>
+    <t>commute = commute2 - "work from home" in denominator</t>
+  </si>
+  <si>
+    <t>Rent50_Severe</t>
+  </si>
+  <si>
+    <t>Park_Access</t>
+  </si>
+  <si>
+    <t>Crowded_House</t>
+  </si>
+  <si>
+    <t>Limited_English</t>
+  </si>
+  <si>
+    <t>Red_Line</t>
+  </si>
+  <si>
+    <t>Extra_Income</t>
+  </si>
+  <si>
+    <t>Food_Affordability</t>
+  </si>
+  <si>
+    <t>HPI_Score</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>neg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +328,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,9 +359,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,71 +680,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF171A8-B713-4052-97AE-66B75AD70E22}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="95.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="95.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>36</v>
       </c>
       <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" t="s">
+      <c r="J1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -651,17 +764,23 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -671,54 +790,66 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" t="s">
         <v>2</v>
       </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -728,157 +859,362 @@
       <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" t="s">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" t="s">
         <v>5</v>
       </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
         <v>44</v>
       </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="J11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
         <v>45</v>
       </c>
-      <c r="H10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="J13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H14" t="s">
         <v>17</v>
       </c>
-      <c r="G13" t="s">
-        <v>48</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I14" t="s">
+        <v>81</v>
+      </c>
+      <c r="J14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" t="s">
         <v>18</v>
       </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="I15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" t="s">
+        <v>83</v>
+      </c>
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" t="s">
+        <v>88</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" t="s">
+        <v>89</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -888,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5A9E1B-9DF5-4584-8522-6E7DBCC083B7}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,6 +1252,11 @@
         <v>35</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CCB October push - Update death data using improved state/county assignment method
</commit_message>
<xml_diff>
--- a/myCCB/Standards/sdohLink.xlsx
+++ b/myCCB/Standards/sdohLink.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2FC1E1-80FA-40E3-9080-0A5F93451F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF0F0BC-C6BD-4BD2-AF03-6383A96C432F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="630" windowWidth="21600" windowHeight="11385" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
+    <workbookView xWindow="0" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="93">
   <si>
     <t>hpi2score</t>
   </si>
@@ -305,6 +305,15 @@
   </si>
   <si>
     <t>neg</t>
+  </si>
+  <si>
+    <t>inSHA_CM</t>
+  </si>
+  <si>
+    <t>poverty150</t>
+  </si>
+  <si>
+    <t>Percentage of population that is Below Federal Poverty Rate of 150%</t>
   </si>
 </sst>
 </file>
@@ -680,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF171A8-B713-4052-97AE-66B75AD70E22}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,15 +700,16 @@
     <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="95.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" customWidth="1"/>
+    <col min="11" max="11" width="95.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -710,51 +720,54 @@
         <v>55</v>
       </c>
       <c r="D1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>87</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
         <v>88</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>86</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -764,23 +777,23 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
         <v>88</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -790,66 +803,69 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" t="s">
         <v>88</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" t="s">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
         <v>89</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>39</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
       </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
         <v>88</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>40</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -859,362 +875,385 @@
       <c r="C7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
         <v>89</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>41</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
         <v>89</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I9" t="s">
         <v>5</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J9" t="s">
         <v>42</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" t="s">
         <v>89</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I10" t="s">
         <v>6</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J10" t="s">
         <v>43</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
         <v>89</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I11" t="s">
         <v>72</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J11" t="s">
         <v>79</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K11" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s">
         <v>88</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I12" t="s">
         <v>7</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J12" t="s">
         <v>44</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" t="s">
         <v>88</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I13" t="s">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J13" t="s">
         <v>80</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
         <v>88</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I14" t="s">
         <v>9</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J14" t="s">
         <v>45</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
         <v>89</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I15" t="s">
         <v>17</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J15" t="s">
         <v>81</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" t="s">
         <v>89</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I16" t="s">
         <v>18</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J16" t="s">
         <v>82</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="H17" t="s">
         <v>89</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I17" t="s">
         <v>56</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J17" t="s">
         <v>83</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>61</v>
       </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" t="s">
         <v>88</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I18" t="s">
         <v>60</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J18" t="s">
         <v>84</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>62</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I19" t="s">
         <v>63</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J19" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" t="s">
         <v>88</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I20" t="s">
         <v>67</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J20" t="s">
         <v>66</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" t="s">
         <v>88</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I21" t="s">
         <v>68</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J21" t="s">
         <v>69</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" t="s">
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" t="s">
         <v>88</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I22" t="s">
         <v>68</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J22" t="s">
         <v>69</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K22" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s">
         <v>89</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I23" t="s">
         <v>74</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J23" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CCB May 2023 Push - Process and add 2022 death data to CCB, and update SHA CM 2023
</commit_message>
<xml_diff>
--- a/myCCB/Standards/sdohLink.xlsx
+++ b/myCCB/Standards/sdohLink.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEED916-7882-416F-9490-E5820D2A897A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B008FD-BA79-460D-BD79-509B1DC45E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8085" yWindow="7245" windowWidth="28800" windowHeight="15435" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="132">
   <si>
     <t>hpi2score</t>
   </si>
@@ -352,9 +352,6 @@
     <t>There are a few SDOH variables that can only be pulled in the positive direction. Estimates going in the negative direction are computed by simple subtracting the estimates by 1.</t>
   </si>
   <si>
-    <t>Not_In_School</t>
-  </si>
-  <si>
     <t>inschool</t>
   </si>
   <si>
@@ -404,6 +401,36 @@
   </si>
   <si>
     <t>Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ICE_Black</t>
+  </si>
+  <si>
+    <t>ICE_Latino</t>
+  </si>
+  <si>
+    <t>iceBlack</t>
+  </si>
+  <si>
+    <t>iceLatino</t>
+  </si>
+  <si>
+    <t>Index of Concentration at the Extremes (ICE) - Compares population counts of White, NH to Black, NH</t>
+  </si>
+  <si>
+    <t>Index of Concentration at the Extremes (ICE) - Compares population counts of White, NH to Hispanics</t>
+  </si>
+  <si>
+    <t>iceBlack [CALCULATED]</t>
+  </si>
+  <si>
+    <t>iceLatino [CALCULATED]</t>
+  </si>
+  <si>
+    <t>Not_In_Pre_School</t>
   </si>
 </sst>
 </file>
@@ -438,12 +465,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -458,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -466,6 +499,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,10 +814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF171A8-B713-4052-97AE-66B75AD70E22}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -879,12 +913,12 @@
         <v>34</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>33</v>
@@ -905,7 +939,7 @@
         <v>93</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -997,13 +1031,13 @@
         <v>79</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1138,13 +1172,13 @@
         <v>80</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J14" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="K14" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1207,10 +1241,10 @@
         <v>7</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1256,7 +1290,7 @@
         <v>100</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1428,10 +1462,10 @@
         <v>59</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1500,7 +1534,7 @@
         <v>102</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1531,25 +1565,71 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="K32" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
April 2024 push - OOS deaths
</commit_message>
<xml_diff>
--- a/myCCB/Standards/sdohLink.xlsx
+++ b/myCCB/Standards/sdohLink.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\Standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB4D197-B90C-4E81-A83B-DFB18CE126AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9463EF-F360-4DB6-AC11-1853A588B4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{510F5D81-3FDD-4905-8CCD-2D26C4177FA0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="159">
   <si>
     <t>hpi2score</t>
   </si>
@@ -502,6 +502,12 @@
   </si>
   <si>
     <t>Crime</t>
+  </si>
+  <si>
+    <t>Total crime index - ESRI</t>
+  </si>
+  <si>
+    <t>Extreme segration - low income Black population - high income White</t>
   </si>
 </sst>
 </file>
@@ -879,7 +885,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,6 +1954,9 @@
       <c r="N37" t="s">
         <v>156</v>
       </c>
+      <c r="O37" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1964,6 +1973,9 @@
       </c>
       <c r="N38" t="s">
         <v>154</v>
+      </c>
+      <c r="O38" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>